<commit_message>
Updated with better calculation and new Prediction Formula
</commit_message>
<xml_diff>
--- a/docs/FunctionPoints_Use-Cases/FunctionPoints_All.xlsx
+++ b/docs/FunctionPoints_Use-Cases/FunctionPoints_All.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Function Points All" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Time (h)</t>
   </si>
@@ -45,10 +45,10 @@
     <t>Use-Case (todo)</t>
   </si>
   <si>
-    <t>?</t>
+    <t>FP (TT)</t>
   </si>
   <si>
-    <t>FP (0 - 11)</t>
+    <t>Time (Calculated)</t>
   </si>
 </sst>
 </file>
@@ -84,11 +84,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -127,7 +128,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -159,7 +160,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -182,8 +183,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.670603674540682E-2"/>
-          <c:y val="0.13436090096581066"/>
+          <c:x val="8.8613579954866156E-2"/>
+          <c:y val="0.16769422572178477"/>
           <c:w val="0.88396062992125979"/>
           <c:h val="0.72088764946048411"/>
         </c:manualLayout>
@@ -200,7 +201,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>FP (0 - 11)</c:v>
+                  <c:v>FP (TT)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -213,8 +214,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -223,54 +224,32 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
+              <a:ln w="9525" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:forward val="4"/>
-            <c:backward val="4"/>
+            <c:forward val="7"/>
+            <c:backward val="2"/>
             <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5472271974586866E-2"/>
+                  <c:y val="-1.4360892388451443E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -284,7 +263,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -305,7 +284,7 @@
             <c:numRef>
               <c:f>'Function Points All'!$C$3:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>12</c:v>
@@ -326,19 +305,19 @@
             <c:numRef>
               <c:f>'Function Points All'!$D$3:$D$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>59.84</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>33.44</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>59.84</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>21.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -347,6 +326,66 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B581-4C82-AC10-8D318DC24D27}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Future</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Function Points All'!$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>17.213333333333335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Function Points All'!$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>93.28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-618A-4502-95B1-0CC8A5E433A6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -382,17 +421,17 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -444,17 +483,17 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -499,7 +538,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -571,7 +610,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -582,7 +621,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -598,25 +637,25 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -628,7 +667,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -636,11 +675,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -672,35 +711,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -712,22 +761,26 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -757,15 +810,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -775,7 +826,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -784,7 +835,43 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -794,65 +881,125 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -865,54 +1012,17 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -922,8 +1032,8 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
+  </cs:seriesLine>
+  <cs:title>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -933,66 +1043,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1001,14 +1052,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1022,27 +1072,26 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1059,9 +1108,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1074,14 +1123,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1090,16 +1133,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1392,13 +1435,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1410,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -1418,48 +1462,52 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
+      <c r="D3" s="2">
+        <v>59.84</v>
+      </c>
+      <c r="E3" s="2"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>9</v>
       </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
+      <c r="D4" s="2">
+        <v>33.44</v>
+      </c>
+      <c r="E4" s="2"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>10</v>
       </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
+      <c r="D5" s="2">
+        <v>59.84</v>
+      </c>
+      <c r="E5" s="2"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
+      <c r="D6" s="2">
+        <v>21.12</v>
+      </c>
+      <c r="E6" s="2"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -1469,14 +1517,24 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
-        <v>8</v>
+      <c r="C9" s="2">
+        <f xml:space="preserve"> (D9+10)/6</f>
+        <v>17.213333333333335</v>
+      </c>
+      <c r="D9" s="2">
+        <v>93.28</v>
       </c>
       <c r="I9" s="1"/>
     </row>

</xml_diff>